<commit_message>
Names Dialog can now be searched
</commit_message>
<xml_diff>
--- a/Defect List.xlsx
+++ b/Defect List.xlsx
@@ -13,17 +13,17 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1580629691" val="973" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1580629691" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1580629691" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1580629691"/>
+      <pm:revision xmlns:pm="smNativeData" day="1580632340" val="973" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1580632340" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1580632340" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1580632340"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Trash icon does not load when slider is moved to closed</t>
   </si>
@@ -38,6 +38,11 @@
   </si>
   <si>
     <t>Remiders are not set right if the app is minimized in the middle of a entru</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[2/2/2020]added bOnPause to taskQEntryActivity </t>
+    </r>
   </si>
   <si>
     <t>check the lowest API we can actually support</t>
@@ -119,7 +124,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1580629691" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1580632340" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -134,7 +139,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1580629691" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1580632340" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -149,7 +154,7 @@
       <sz val="9"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1580629691" fgClr="E8BF6A" bgClr="A9B7C6" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1580632340" fgClr="E8BF6A" bgClr="A9B7C6" ulstyle="none">
             <pm:latin face="Bitstream Vera Sans Mono" sz="180" lang="default"/>
             <pm:cs face="Basic Sans" sz="180" lang="default"/>
             <pm:ea face="Basic Sans" sz="180" lang="default"/>
@@ -164,7 +169,7 @@
       <sz val="9"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1580629691" fgClr="BABABA" bgClr="A9B7C6" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1580632340" fgClr="BABABA" bgClr="A9B7C6" ulstyle="none">
             <pm:latin face="Bitstream Vera Sans Mono" sz="180" lang="default"/>
             <pm:cs face="Basic Sans" sz="180" lang="default"/>
             <pm:ea face="Basic Sans" sz="180" lang="default"/>
@@ -179,7 +184,7 @@
       <sz val="9"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1580629691" fgClr="BABABA" bgClr="A9B7C6" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1580632340" fgClr="BABABA" bgClr="A9B7C6" ulstyle="none">
             <pm:latin face="Bitstream Vera Sans Mono" sz="180" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -201,7 +206,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1580629691" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1580632340" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -223,7 +228,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1580629691"/>
+          <pm:border xmlns:pm="smNativeData" id="1580632340"/>
         </ext>
       </extLst>
     </border>
@@ -242,7 +247,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1580629691"/>
+          <pm:border xmlns:pm="smNativeData" id="1580632340"/>
         </ext>
       </extLst>
     </border>
@@ -263,10 +268,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1580629691" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1580632340" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1580629691" count="6">
+      <pm:colors xmlns:pm="smNativeData" id="1580632340" count="6">
         <pm:color name="Color 26" rgb="E8BF6A"/>
         <pm:color name="Color 24" rgb="A9B7C6"/>
         <pm:color name="Color 25" rgb="2B2B2B"/>
@@ -537,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:C79"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
@@ -569,12 +574,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4" t="n">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -582,7 +590,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -590,7 +598,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -598,7 +606,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -606,7 +614,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -614,7 +622,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -622,7 +630,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -630,7 +638,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -638,7 +646,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -646,7 +654,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -654,7 +662,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -662,7 +670,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -670,7 +678,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -678,7 +686,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -686,7 +694,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -694,7 +702,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -702,7 +710,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -710,7 +718,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -718,7 +726,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -726,7 +734,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:1">
@@ -1015,7 +1023,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1580629691" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1580632340" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1024,14 +1032,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1580629691" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1580629691" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1580632340" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1580632340" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1580629691" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1580632340" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Save and Cancel buttons added. Names dialog sets focus on search on load.
</commit_message>
<xml_diff>
--- a/Defect List.xlsx
+++ b/Defect List.xlsx
@@ -13,17 +13,17 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1580632340" val="973" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1580632340" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1580632340" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1580632340"/>
+      <pm:revision xmlns:pm="smNativeData" day="1580639039" val="973" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1580639039" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1580639039" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1580639039"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Trash icon does not load when slider is moved to closed</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>search not working in names list</t>
+  </si>
+  <si>
+    <t>[2/2/2020]Fixed</t>
   </si>
   <si>
     <t>sort what and who lists by count</t>
@@ -124,7 +127,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1580632340" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1580639039" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -139,7 +142,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1580632340" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1580639039" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -154,7 +157,7 @@
       <sz val="9"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1580632340" fgClr="E8BF6A" bgClr="A9B7C6" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1580639039" fgClr="E8BF6A" bgClr="A9B7C6" ulstyle="none">
             <pm:latin face="Bitstream Vera Sans Mono" sz="180" lang="default"/>
             <pm:cs face="Basic Sans" sz="180" lang="default"/>
             <pm:ea face="Basic Sans" sz="180" lang="default"/>
@@ -169,7 +172,7 @@
       <sz val="9"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1580632340" fgClr="BABABA" bgClr="A9B7C6" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1580639039" fgClr="BABABA" bgClr="A9B7C6" ulstyle="none">
             <pm:latin face="Bitstream Vera Sans Mono" sz="180" lang="default"/>
             <pm:cs face="Basic Sans" sz="180" lang="default"/>
             <pm:ea face="Basic Sans" sz="180" lang="default"/>
@@ -184,7 +187,7 @@
       <sz val="9"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1580632340" fgClr="BABABA" bgClr="A9B7C6" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1580639039" fgClr="BABABA" bgClr="A9B7C6" ulstyle="none">
             <pm:latin face="Bitstream Vera Sans Mono" sz="180" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -206,7 +209,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1580632340" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1580639039" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -228,7 +231,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1580632340"/>
+          <pm:border xmlns:pm="smNativeData" id="1580639039"/>
         </ext>
       </extLst>
     </border>
@@ -247,7 +250,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1580632340"/>
+          <pm:border xmlns:pm="smNativeData" id="1580639039"/>
         </ext>
       </extLst>
     </border>
@@ -268,10 +271,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1580632340" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1580639039" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1580632340" count="6">
+      <pm:colors xmlns:pm="smNativeData" id="1580639039" count="6">
         <pm:color name="Color 26" rgb="E8BF6A"/>
         <pm:color name="Color 24" rgb="A9B7C6"/>
         <pm:color name="Color 25" rgb="2B2B2B"/>
@@ -542,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:C79"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
@@ -601,12 +604,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:3">
       <c r="A7" t="n">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -614,7 +620,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -622,7 +628,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -630,7 +636,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -638,7 +644,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -646,7 +652,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -654,7 +660,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -662,7 +668,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -670,7 +676,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -678,7 +684,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -686,7 +692,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -694,7 +700,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -702,7 +708,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -710,7 +716,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -718,7 +724,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -726,7 +732,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -734,7 +740,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:1">
@@ -1023,7 +1029,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1580632340" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1580639039" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1032,14 +1038,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1580632340" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1580632340" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1580639039" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1580639039" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1580632340" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1580639039" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Fixed bug 12 - if you save task without tags, you get a empty tags dialog afterwards and reminder time kees resetting to current time
</commit_message>
<xml_diff>
--- a/Defect List.xlsx
+++ b/Defect List.xlsx
@@ -13,17 +13,17 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1580639039" val="973" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1580639039" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1580639039" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1580639039"/>
+      <pm:revision xmlns:pm="smNativeData" day="1580644151" val="973" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1580644151" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1580644151" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1580644151"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Trash icon does not load when slider is moved to closed</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>add option to cancel edit on a task</t>
+  </si>
+  <si>
+    <t>[2/2/2020]Done</t>
   </si>
   <si>
     <t>if you save task without tags, you get a empty tags dialog afterwards and reminder time kees resetting to current time</t>
@@ -127,7 +130,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1580639039" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1580644151" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -142,7 +145,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1580639039" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1580644151" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -157,7 +160,7 @@
       <sz val="9"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1580639039" fgClr="E8BF6A" bgClr="A9B7C6" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1580644151" fgClr="E8BF6A" bgClr="A9B7C6" ulstyle="none">
             <pm:latin face="Bitstream Vera Sans Mono" sz="180" lang="default"/>
             <pm:cs face="Basic Sans" sz="180" lang="default"/>
             <pm:ea face="Basic Sans" sz="180" lang="default"/>
@@ -172,7 +175,7 @@
       <sz val="9"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1580639039" fgClr="BABABA" bgClr="A9B7C6" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1580644151" fgClr="BABABA" bgClr="A9B7C6" ulstyle="none">
             <pm:latin face="Bitstream Vera Sans Mono" sz="180" lang="default"/>
             <pm:cs face="Basic Sans" sz="180" lang="default"/>
             <pm:ea face="Basic Sans" sz="180" lang="default"/>
@@ -187,7 +190,7 @@
       <sz val="9"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1580639039" fgClr="BABABA" bgClr="A9B7C6" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1580644151" fgClr="BABABA" bgClr="A9B7C6" ulstyle="none">
             <pm:latin face="Bitstream Vera Sans Mono" sz="180" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -209,7 +212,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1580639039" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1580644151" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -231,7 +234,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1580639039"/>
+          <pm:border xmlns:pm="smNativeData" id="1580644151"/>
         </ext>
       </extLst>
     </border>
@@ -250,7 +253,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1580639039"/>
+          <pm:border xmlns:pm="smNativeData" id="1580644151"/>
         </ext>
       </extLst>
     </border>
@@ -271,10 +274,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1580639039" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1580644151" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1580639039" count="6">
+      <pm:colors xmlns:pm="smNativeData" id="1580644151" count="6">
         <pm:color name="Color 26" rgb="E8BF6A"/>
         <pm:color name="Color 24" rgb="A9B7C6"/>
         <pm:color name="Color 25" rgb="2B2B2B"/>
@@ -546,7 +549,7 @@
   <dimension ref="A2:C79"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
@@ -639,19 +642,25 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:3">
       <c r="A11" t="n">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="n">
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
         <v>14</v>
       </c>
     </row>
@@ -660,7 +669,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -668,7 +677,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -676,7 +685,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -684,7 +693,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -692,7 +701,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -700,7 +709,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -708,7 +717,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -716,7 +725,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -724,7 +733,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -732,7 +741,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -740,7 +749,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:1">
@@ -1029,7 +1038,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1580639039" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1580644151" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1038,14 +1047,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1580639039" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1580639039" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1580644151" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1580644151" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1580639039" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1580644151" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Fixed bug 18 - add preset reminder times such as morning, start of workday, end of workday, after dinner - added partial fix with hard coded values
</commit_message>
<xml_diff>
--- a/Defect List.xlsx
+++ b/Defect List.xlsx
@@ -13,17 +13,17 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1580644151" val="973" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1580644151" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1580644151" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1580644151"/>
+      <pm:revision xmlns:pm="smNativeData" day="1580648266" val="973" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1580648266" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1580648266" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1580648266"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>Trash icon does not load when slider is moved to closed</t>
   </si>
@@ -40,9 +40,7 @@
     <t>Remiders are not set right if the app is minimized in the middle of a entru</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">[2/2/2020]added bOnPause to taskQEntryActivity </t>
-    </r>
+    <t xml:space="preserve">[2/2/2020]added bOnPause to taskQEntryActivity </t>
   </si>
   <si>
     <t>check the lowest API we can actually support</t>
@@ -90,10 +88,16 @@
     <t>StrSeparator shows up in reminders</t>
   </si>
   <si>
+    <t>[2/2/2020]Could not recreate</t>
+  </si>
+  <si>
     <t>feilds reset after a tags/names dialog</t>
   </si>
   <si>
     <t>add preset reminder times such as morning, start of workday, end of workday, after dinner</t>
+  </si>
+  <si>
+    <t>[2/2/2020]Added hardcoded values</t>
   </si>
   <si>
     <t>reminder of deleted tasks show up</t>
@@ -122,7 +126,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₹&quot;_-;\-* #,##0.00\ &quot;₹&quot;_-;_-* &quot;-&quot;??\ &quot;₹&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₹_-;\-* #,##0.00\ _₹_-;_-* &quot;-&quot;??\ _₹_-;_-@_-"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <name val="Arial"/>
       <family val="2"/>
@@ -130,7 +134,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1580644151" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1580648266" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -145,7 +149,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1580644151" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1580648266" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -160,40 +164,10 @@
       <sz val="9"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1580644151" fgClr="E8BF6A" bgClr="A9B7C6" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1580648266" fgClr="E8BF6A" bgClr="A9B7C6" ulstyle="none">
             <pm:latin face="Bitstream Vera Sans Mono" sz="180" lang="default"/>
             <pm:cs face="Basic Sans" sz="180" lang="default"/>
             <pm:ea face="Basic Sans" sz="180" lang="default"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
-    </font>
-    <font>
-      <name val="Bitstream Vera Sans Mono"/>
-      <family val="1"/>
-      <color rgb="FFBABABA"/>
-      <sz val="9"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1580644151" fgClr="BABABA" bgClr="A9B7C6" ulstyle="none">
-            <pm:latin face="Bitstream Vera Sans Mono" sz="180" lang="default"/>
-            <pm:cs face="Basic Sans" sz="180" lang="default"/>
-            <pm:ea face="Basic Sans" sz="180" lang="default"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
-    </font>
-    <font>
-      <name val="Bitstream Vera Sans Mono"/>
-      <family val="1"/>
-      <color rgb="FFBABABA"/>
-      <sz val="9"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1580644151" fgClr="BABABA" bgClr="A9B7C6" ulstyle="none">
-            <pm:latin face="Bitstream Vera Sans Mono" sz="180" lang="default"/>
-            <pm:cs face="Times New Roman" sz="200" lang="default"/>
-            <pm:ea face="SimSun" sz="200" lang="default"/>
           </pm:charSpec>
         </ext>
       </extLst>
@@ -212,7 +186,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1580644151" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1580648266" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -234,7 +208,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1580644151"/>
+          <pm:border xmlns:pm="smNativeData" id="1580648266"/>
         </ext>
       </extLst>
     </border>
@@ -253,7 +227,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1580644151"/>
+          <pm:border xmlns:pm="smNativeData" id="1580648266"/>
         </ext>
       </extLst>
     </border>
@@ -274,10 +248,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1580644151" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1580648266" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1580644151" count="6">
+      <pm:colors xmlns:pm="smNativeData" id="1580648266" count="6">
         <pm:color name="Color 26" rgb="E8BF6A"/>
         <pm:color name="Color 24" rgb="A9B7C6"/>
         <pm:color name="Color 25" rgb="2B2B2B"/>
@@ -549,13 +523,13 @@
   <dimension ref="A2:C79"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
   <cols>
     <col min="2" max="2" width="94.099099" customWidth="1"/>
-    <col min="3" max="3" width="80.135135" customWidth="1"/>
+    <col min="3" max="3" width="56.216216" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3">
@@ -680,12 +654,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:3">
       <c r="A15" t="n">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -696,28 +673,37 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:3">
       <c r="A17" t="n">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="n">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="n">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -725,15 +711,18 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="n">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -741,7 +730,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -749,7 +738,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:1">
@@ -1038,7 +1027,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1580644151" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1580648266" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1047,14 +1036,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1580644151" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1580644151" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1580648266" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1580648266" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1580644151" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1580648266" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>